<commit_message>
Locator change in pre-release
</commit_message>
<xml_diff>
--- a/ExcelFiles/MedicalCertificate.xlsx
+++ b/ExcelFiles/MedicalCertificate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0419B7C-FFDB-4311-A7FA-8B82B942EFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7294CF-5D58-42F4-944C-F3207839888A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
     <t>01-04-2025</t>
   </si>
   <si>
-    <t>30-07-2025</t>
+    <t>30-08-2025</t>
   </si>
 </sst>
 </file>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EA1B80-280E-4D26-AF18-E86A7C091F1D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DCC597-3277-451D-BCC4-5E31042A1E67}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1951,15 +1951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -2214,6 +2205,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2226,14 +2226,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4E55A-6C67-4895-94E6-14C6B175BE34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCB7D6A-E6F4-49F1-91EA-99C5773FBF86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2252,6 +2244,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4E55A-6C67-4895-94E6-14C6B175BE34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E45471CC-9AFA-4147-A50A-01BCBC520F94}">
   <ds:schemaRefs>

</xml_diff>